<commit_message>
added feed firmware documentation
</commit_message>
<xml_diff>
--- a/Antonio-Feed/Documents/Feed Manual/Feed Control Commands 6.0.xlsx
+++ b/Antonio-Feed/Documents/Feed Manual/Feed Control Commands 6.0.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pollak/Documents/GitHub/Front-Page/Antonio-Feed/Documents/Feed Manual/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A52166A9-D710-2648-88E1-B1207228D0AF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F90729C-CCD6-8E41-9DF9-86F7F3C70627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-47540" yWindow="2180" windowWidth="28040" windowHeight="17440" xr2:uid="{558E7373-39A1-AA44-8449-14843B753A0F}"/>
+    <workbookView xWindow="-72660" yWindow="2400" windowWidth="28040" windowHeight="17440" xr2:uid="{558E7373-39A1-AA44-8449-14843B753A0F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="130">
   <si>
     <t>Feed Control Board Commands V6.0</t>
   </si>
@@ -429,6 +429,15 @@
   </si>
   <si>
     <t>Display parameters stored in memory</t>
+  </si>
+  <si>
+    <t>Moves the auto start program to the next step</t>
+  </si>
+  <si>
+    <t>str (Move to step XX)</t>
+  </si>
+  <si>
+    <t>step</t>
   </si>
 </sst>
 </file>
@@ -509,31 +518,28 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -868,10 +874,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{991E4D36-F9F0-A34B-8953-2AEE2AB1F790}">
-  <dimension ref="A1:F88"/>
+  <dimension ref="A1:F89"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B75" sqref="B75"/>
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -884,33 +890,33 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
     </row>
     <row r="2" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="3" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F3" s="3"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
@@ -922,10 +928,10 @@
       <c r="C4" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="4"/>
+      <c r="F4" s="8"/>
     </row>
     <row r="5" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
@@ -937,10 +943,10 @@
       <c r="C5" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="8" t="s">
+      <c r="E5" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="6"/>
     </row>
     <row r="6" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
@@ -1031,16 +1037,13 @@
         <v>9</v>
       </c>
       <c r="B12" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="C12" t="s">
-        <v>122</v>
-      </c>
-      <c r="D12" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="F12" s="6"/>
     </row>
@@ -1049,7 +1052,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C13" t="s">
         <v>122</v>
@@ -1058,7 +1061,7 @@
         <v>122</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F13" s="6"/>
     </row>
@@ -1067,7 +1070,7 @@
         <v>11</v>
       </c>
       <c r="B14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C14" t="s">
         <v>122</v>
@@ -1076,42 +1079,44 @@
         <v>122</v>
       </c>
       <c r="E14" s="6" t="s">
+        <v>124</v>
+      </c>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C15" t="s">
+        <v>122</v>
+      </c>
+      <c r="D15" t="s">
+        <v>122</v>
+      </c>
+      <c r="E15" s="6" t="s">
         <v>126</v>
       </c>
-      <c r="F14" s="6"/>
-    </row>
-    <row r="15" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1">
-        <v>12</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D16" s="5"/>
-      <c r="E16" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F16" s="6"/>
+      <c r="A16" s="1"/>
     </row>
     <row r="17" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>13</v>
       </c>
       <c r="B17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C17" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="5"/>
+      <c r="D17" s="3"/>
       <c r="E17" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F17" s="6"/>
     </row>
@@ -1120,14 +1125,14 @@
         <v>14</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
-      </c>
-      <c r="C18" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D18" s="5"/>
+      <c r="D18" s="3"/>
       <c r="E18" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F18" s="6"/>
     </row>
@@ -1136,14 +1141,14 @@
         <v>15</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
-      </c>
-      <c r="C19" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C19" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D19" s="5"/>
+      <c r="D19" s="3"/>
       <c r="E19" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F19" s="6"/>
     </row>
@@ -1152,14 +1157,14 @@
         <v>16</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
-      </c>
-      <c r="C20" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="5"/>
+      <c r="D20" s="3"/>
       <c r="E20" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F20" s="6"/>
     </row>
@@ -1168,14 +1173,14 @@
         <v>17</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
-      </c>
-      <c r="C21" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D21" s="5"/>
+      <c r="D21" s="3"/>
       <c r="E21" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F21" s="6"/>
     </row>
@@ -1184,49 +1189,49 @@
         <v>18</v>
       </c>
       <c r="B22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F22" s="6"/>
+    </row>
+    <row r="23" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>19</v>
+      </c>
+      <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="5" t="s">
+      <c r="C23" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D22" s="5"/>
-      <c r="E22" s="6" t="s">
+      <c r="D23" s="3"/>
+      <c r="E23" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="6"/>
-    </row>
-    <row r="23" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
+      <c r="F23" s="6"/>
     </row>
     <row r="24" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1">
-        <v>19</v>
-      </c>
-      <c r="B24" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" s="5"/>
-      <c r="E24" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="F24" s="6"/>
+      <c r="A24" s="1"/>
     </row>
     <row r="25" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>20</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
-      </c>
-      <c r="C25" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D25" s="5"/>
+      <c r="D25" s="3"/>
       <c r="E25" s="6" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="F25" s="6"/>
     </row>
@@ -1235,14 +1240,14 @@
         <v>21</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
-      </c>
-      <c r="C26" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="5"/>
+      <c r="D26" s="3"/>
       <c r="E26" s="6" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="F26" s="6"/>
     </row>
@@ -1251,14 +1256,14 @@
         <v>22</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D27" s="5"/>
+      <c r="D27" s="3"/>
       <c r="E27" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F27" s="6"/>
     </row>
@@ -1267,14 +1272,14 @@
         <v>23</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
-      </c>
-      <c r="C28" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D28" s="5"/>
+      <c r="D28" s="3"/>
       <c r="E28" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F28" s="6"/>
     </row>
@@ -1283,14 +1288,14 @@
         <v>24</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
-      </c>
-      <c r="C29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D29" s="5"/>
+      <c r="D29" s="3"/>
       <c r="E29" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F29" s="6"/>
     </row>
@@ -1299,49 +1304,49 @@
         <v>25</v>
       </c>
       <c r="B30" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="3"/>
+      <c r="E30" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="6"/>
+    </row>
+    <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>26</v>
+      </c>
+      <c r="B31" t="s">
         <v>32</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="C31" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D30" s="5"/>
-      <c r="E30" s="6" t="s">
+      <c r="D31" s="3"/>
+      <c r="E31" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="F30" s="6"/>
-    </row>
-    <row r="31" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1">
-        <v>26</v>
-      </c>
-      <c r="B32" t="s">
-        <v>33</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D32" s="5"/>
-      <c r="E32" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F32" s="6"/>
-    </row>
-    <row r="33" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="6"/>
+    </row>
+    <row r="32" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="1"/>
+    </row>
+    <row r="33" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>27</v>
       </c>
       <c r="B33" t="s">
-        <v>34</v>
-      </c>
-      <c r="C33" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D33" s="5"/>
-      <c r="E33" s="6" t="s">
-        <v>44</v>
+      <c r="D33" s="3"/>
+      <c r="E33" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="F33" s="6"/>
     </row>
@@ -1350,14 +1355,14 @@
         <v>28</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
-      </c>
-      <c r="C34" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D34" s="5"/>
+        <v>34</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D34" s="3"/>
       <c r="E34" s="6" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="F34" s="6"/>
     </row>
@@ -1365,35 +1370,36 @@
       <c r="A35" s="1">
         <v>29</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B35" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D35" s="3"/>
+      <c r="E35" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>30</v>
       </c>
-      <c r="B36" t="s">
-        <v>39</v>
-      </c>
-      <c r="C36" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="5"/>
-      <c r="E36" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="F36" s="6"/>
-    </row>
-    <row r="37" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="37" spans="1:6" ht="72" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>31</v>
       </c>
       <c r="B37" t="s">
-        <v>42</v>
-      </c>
-      <c r="C37" t="s">
+        <v>39</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>43</v>
+      <c r="D37" s="3"/>
+      <c r="E37" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="F37" s="6"/>
     </row>
@@ -1402,68 +1408,67 @@
         <v>32</v>
       </c>
       <c r="B38" t="s">
+        <v>42</v>
+      </c>
+      <c r="C38" t="s">
+        <v>41</v>
+      </c>
+      <c r="E38" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>33</v>
+      </c>
+      <c r="B39" t="s">
         <v>45</v>
       </c>
-      <c r="C38" s="5" t="s">
+      <c r="C39" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="D38" s="5"/>
-      <c r="E38" s="6" t="s">
+      <c r="D39" s="3"/>
+      <c r="E39" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="F38" s="6"/>
-    </row>
-    <row r="39" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1">
-        <v>33</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="1"/>
+    </row>
+    <row r="41" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="1">
+        <v>34</v>
+      </c>
+      <c r="B41" t="s">
         <v>47</v>
       </c>
-      <c r="C40" s="5" t="s">
+      <c r="C41" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="D40" s="5"/>
-      <c r="E40" s="7" t="s">
+      <c r="D41" s="3"/>
+      <c r="E41" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="F40" s="6"/>
-    </row>
-    <row r="41" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
+      <c r="F41" s="6"/>
     </row>
     <row r="42" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1">
-        <v>34</v>
-      </c>
-      <c r="B42" t="s">
-        <v>50</v>
-      </c>
-      <c r="C42" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="D42" s="5"/>
-      <c r="E42" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="F42" s="6"/>
+      <c r="A42" s="1"/>
     </row>
     <row r="43" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>35</v>
       </c>
       <c r="B43" t="s">
-        <v>52</v>
-      </c>
-      <c r="C43" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D43" s="5"/>
+      <c r="D43" s="3"/>
       <c r="E43" s="6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F43" s="6"/>
     </row>
@@ -1471,346 +1476,359 @@
       <c r="A44" s="1">
         <v>36</v>
       </c>
+      <c r="B44" t="s">
+        <v>52</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" s="3"/>
+      <c r="E44" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="F44" s="6"/>
     </row>
     <row r="45" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1">
+      <c r="A45" s="1"/>
+    </row>
+    <row r="46" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="1">
         <v>37</v>
       </c>
-      <c r="B45" t="s">
+      <c r="B46" t="s">
         <v>58</v>
       </c>
-      <c r="C45" s="5" t="s">
+      <c r="C46" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="5"/>
-      <c r="E45" s="6" t="s">
+      <c r="D46" s="3"/>
+      <c r="E46" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="F45" s="6"/>
-    </row>
-    <row r="46" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1">
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
         <v>38</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B47" t="s">
         <v>61</v>
       </c>
-      <c r="D46" t="s">
+      <c r="D47" t="s">
         <v>88</v>
       </c>
-      <c r="E46" s="7" t="s">
+      <c r="E47" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="F46" s="6"/>
-    </row>
-    <row r="47" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1">
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
         <v>39</v>
       </c>
-      <c r="B47" t="s">
+      <c r="B48" t="s">
         <v>64</v>
       </c>
-      <c r="C47" s="5" t="s">
+      <c r="C48" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="E47" s="6" t="s">
+      <c r="E48" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="F47" s="6"/>
-    </row>
-    <row r="48" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1">
-        <v>40</v>
-      </c>
-      <c r="B49" t="s">
-        <v>68</v>
-      </c>
-      <c r="C49" t="s">
-        <v>69</v>
-      </c>
-      <c r="E49" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="F49" s="6"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="1"/>
     </row>
     <row r="50" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
+        <v>40</v>
+      </c>
+      <c r="B50" t="s">
+        <v>68</v>
+      </c>
+      <c r="C50" t="s">
+        <v>69</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>67</v>
+      </c>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="1">
         <v>41</v>
       </c>
-      <c r="B50" t="s">
+      <c r="B51" t="s">
         <v>70</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C51" t="s">
         <v>71</v>
       </c>
-      <c r="E50" s="7" t="s">
+      <c r="E51" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F50" s="6"/>
-    </row>
-    <row r="51" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="52" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1">
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
         <v>42</v>
       </c>
-      <c r="B52" t="s">
+      <c r="B53" t="s">
         <v>79</v>
       </c>
-      <c r="E52" s="6" t="s">
+      <c r="E53" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="F52" s="6"/>
-    </row>
-    <row r="53" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="E53" s="6"/>
       <c r="F53" s="6"/>
     </row>
-    <row r="54" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1">
-        <v>43</v>
-      </c>
-      <c r="B54" t="s">
-        <v>113</v>
-      </c>
-      <c r="C54" t="s">
-        <v>97</v>
-      </c>
-      <c r="E54" s="7" t="s">
-        <v>115</v>
-      </c>
+    <row r="54" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E54" s="6"/>
       <c r="F54" s="6"/>
     </row>
     <row r="55" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B55" t="s">
-        <v>112</v>
-      </c>
-      <c r="D55" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="C55" t="s">
         <v>97</v>
       </c>
-      <c r="E55" s="7" t="s">
-        <v>114</v>
+      <c r="E55" s="5" t="s">
+        <v>115</v>
       </c>
       <c r="F55" s="6"/>
     </row>
     <row r="56" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B56" t="s">
-        <v>104</v>
-      </c>
-      <c r="C56" t="s">
+        <v>112</v>
+      </c>
+      <c r="D56" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E56" s="7" t="s">
-        <v>106</v>
+      <c r="E56" s="5" t="s">
+        <v>114</v>
       </c>
       <c r="F56" s="6"/>
     </row>
     <row r="57" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B57" t="s">
-        <v>105</v>
-      </c>
-      <c r="D57" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C57" t="s">
         <v>97</v>
       </c>
-      <c r="E57" s="7" t="s">
-        <v>107</v>
+      <c r="E57" s="5" t="s">
+        <v>106</v>
       </c>
       <c r="F57" s="6"/>
     </row>
     <row r="58" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B58" t="s">
-        <v>108</v>
-      </c>
-      <c r="C58" t="s">
+        <v>105</v>
+      </c>
+      <c r="D58" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="D58" s="9"/>
-      <c r="E58" s="7" t="s">
-        <v>110</v>
-      </c>
-      <c r="F58" s="7"/>
+      <c r="E58" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="F58" s="6"/>
     </row>
     <row r="59" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B59" t="s">
-        <v>109</v>
-      </c>
-      <c r="D59" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="C59" t="s">
         <v>97</v>
       </c>
-      <c r="E59" s="7" t="s">
-        <v>111</v>
-      </c>
-      <c r="F59" s="7"/>
+      <c r="D59" s="4"/>
+      <c r="E59" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="F59" s="5"/>
     </row>
     <row r="60" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
+        <v>48</v>
+      </c>
+      <c r="B60" t="s">
+        <v>109</v>
+      </c>
+      <c r="D60" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="E60" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="F60" s="5"/>
+    </row>
+    <row r="61" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
         <v>49</v>
       </c>
-      <c r="B60" t="s">
+      <c r="B61" t="s">
         <v>84</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C61" t="s">
         <v>86</v>
       </c>
-      <c r="E60" s="7" t="s">
+      <c r="E61" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="F60" s="6"/>
-    </row>
-    <row r="61" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1">
-        <v>50</v>
-      </c>
-      <c r="B61" t="s">
-        <v>85</v>
-      </c>
-      <c r="D61" t="s">
-        <v>89</v>
-      </c>
-      <c r="E61" s="6" t="s">
-        <v>90</v>
       </c>
       <c r="F61" s="6"/>
     </row>
     <row r="62" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B62" t="s">
-        <v>91</v>
-      </c>
-      <c r="C62" t="s">
-        <v>97</v>
+        <v>85</v>
+      </c>
+      <c r="D62" t="s">
+        <v>89</v>
       </c>
       <c r="E62" s="6" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="F62" s="6"/>
     </row>
     <row r="63" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
-      </c>
-      <c r="D63" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="C63" t="s">
         <v>97</v>
       </c>
       <c r="E63" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F63" s="6"/>
     </row>
     <row r="64" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B64" t="s">
-        <v>93</v>
-      </c>
-      <c r="C64" t="s">
+        <v>92</v>
+      </c>
+      <c r="D64" s="4" t="s">
         <v>97</v>
       </c>
       <c r="E64" s="6" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="F64" s="6"/>
     </row>
     <row r="65" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B65" t="s">
-        <v>94</v>
-      </c>
-      <c r="D65" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C65" t="s">
         <v>97</v>
       </c>
       <c r="E65" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F65" s="6"/>
     </row>
     <row r="66" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B66" t="s">
-        <v>95</v>
-      </c>
-      <c r="C66" t="s">
+        <v>94</v>
+      </c>
+      <c r="D66" s="4" t="s">
         <v>97</v>
       </c>
       <c r="E66" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="F66" s="6"/>
     </row>
     <row r="67" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
+        <v>55</v>
+      </c>
+      <c r="B67" t="s">
+        <v>95</v>
+      </c>
+      <c r="C67" t="s">
+        <v>97</v>
+      </c>
+      <c r="E67" s="6" t="s">
+        <v>99</v>
+      </c>
+      <c r="F67" s="6"/>
+    </row>
+    <row r="68" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
         <v>56</v>
       </c>
-      <c r="B67" t="s">
+      <c r="B68" t="s">
         <v>96</v>
       </c>
-      <c r="D67" s="9" t="s">
+      <c r="D68" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E67" s="6" t="s">
+      <c r="E68" s="6" t="s">
         <v>100</v>
       </c>
-      <c r="F67" s="6"/>
-    </row>
-    <row r="68" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1">
-        <v>57</v>
-      </c>
-      <c r="B69" t="s">
-        <v>117</v>
-      </c>
-      <c r="C69" t="s">
-        <v>97</v>
-      </c>
-      <c r="E69" s="7" t="s">
-        <v>119</v>
-      </c>
-      <c r="F69" s="6"/>
-    </row>
+      <c r="F68" s="6"/>
+    </row>
+    <row r="69" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="70" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
+        <v>57</v>
+      </c>
+      <c r="B70" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" t="s">
+        <v>97</v>
+      </c>
+      <c r="E70" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="F70" s="6"/>
+    </row>
+    <row r="71" spans="1:6" ht="48" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="1">
         <v>58</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B71" t="s">
         <v>116</v>
       </c>
-      <c r="D70" t="s">
+      <c r="D71" t="s">
         <v>97</v>
       </c>
-      <c r="E70" s="7" t="s">
+      <c r="E71" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="F70" s="6"/>
-    </row>
-    <row r="71" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="F71" s="6"/>
+    </row>
     <row r="72" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="73" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="74" spans="1:6" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1828,66 +1846,68 @@
     <row r="86" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="87" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="88" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="24" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
-  <mergeCells count="58">
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="E70:F70"/>
+  <mergeCells count="59">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="E18:F18"/>
     <mergeCell ref="E12:F12"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E58:F58"/>
-    <mergeCell ref="E59:F59"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E60:F60"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E64:F64"/>
-    <mergeCell ref="E66:F66"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E65:F65"/>
-    <mergeCell ref="E63:F63"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E52:F52"/>
-    <mergeCell ref="E42:F42"/>
-    <mergeCell ref="E43:F43"/>
     <mergeCell ref="E5:F5"/>
     <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E45:F45"/>
     <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E47:F47"/>
     <mergeCell ref="E7:F7"/>
     <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E35:F35"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E40:F40"/>
-    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E39:F39"/>
+    <mergeCell ref="E41:F41"/>
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="E28:F28"/>
     <mergeCell ref="E29:F29"/>
     <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E43:F43"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E33:F33"/>
     <mergeCell ref="E20:F20"/>
     <mergeCell ref="E21:F21"/>
     <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E24:F24"/>
+    <mergeCell ref="E23:F23"/>
     <mergeCell ref="E25:F25"/>
-    <mergeCell ref="A1:F1"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E16:F16"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E66:F66"/>
+    <mergeCell ref="E64:F64"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="E51:F51"/>
+    <mergeCell ref="E70:F70"/>
+    <mergeCell ref="E71:F71"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E58:F58"/>
+    <mergeCell ref="E59:F59"/>
+    <mergeCell ref="E60:F60"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E63:F63"/>
+    <mergeCell ref="E65:F65"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>